<commit_message>
chore: update excel sheet
</commit_message>
<xml_diff>
--- a/src/assets/images/excel-competences.xlsx
+++ b/src/assets/images/excel-competences.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flori\OneDrive - Ifag Paris\Epsi\B2\Cours\Portfolio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ifagparis-my.sharepoint.com/personal/florimond_jaulin_epsi_fr/Documents/Epsi/B2/Cours/Portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A01EED7-DB83-48D6-827E-54E77F39449D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{7A01EED7-DB83-48D6-827E-54E77F39449D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D3C2B02-9AC0-44D4-97F1-F5687E6DE7CE}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$34</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -195,9 +195,6 @@
     <t>Gérer les sauvegardes du code avec Git/GitLab</t>
   </si>
   <si>
-    <t>Suivit d'un maquette pour réaliser le site web conforme aux attentes de l'organisation</t>
-  </si>
-  <si>
     <t>Mise en place d'une sécurisation de l'api avec un jeton JWT</t>
   </si>
   <si>
@@ -228,6 +225,36 @@
   <si>
     <t>dec-21
 avr-22</t>
+  </si>
+  <si>
+    <t>Installation de mon environnement de développement sur un ordinateur professionnel</t>
+  </si>
+  <si>
+    <t>Projet tranversal application  web camping php/mysql</t>
+  </si>
+  <si>
+    <t>Installation de mon environnement de développement sur mon ordinateur personnel</t>
+  </si>
+  <si>
+    <t>Réalisation de tests Gherkin</t>
+  </si>
+  <si>
+    <t>Ajout d'une rubrique d'information sur l'application web 'Matrice de performance'</t>
+  </si>
+  <si>
+    <t>Gestion de mon profil linkedIn</t>
+  </si>
+  <si>
+    <t>Suivi de formations en lien avec mon projet professionnel</t>
+  </si>
+  <si>
+    <t>Suivi d'un maquette pour réaliser le site web conforme aux attentes de l'organisation</t>
+  </si>
+  <si>
+    <t>Réalisation d'un diagramme de Gant</t>
+  </si>
+  <si>
+    <t>Deuxième projet hopital (application mobile) réalisation à partir de maquettes</t>
   </si>
 </sst>
 </file>
@@ -828,15 +855,51 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -869,42 +932,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1248,10 +1275,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AQ80"/>
+  <dimension ref="A1:AQ89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
@@ -1266,56 +1293,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="32"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" s="45"/>
-      <c r="H3" s="51"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="36"/>
+      <c r="H3" s="42"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="49"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="40"/>
       <c r="F4" s="12" t="s">
         <v>8</v>
       </c>
@@ -1327,22 +1354,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="43"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="55"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="51" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1365,8 +1392,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1">
-      <c r="A7" s="31"/>
-      <c r="B7" s="40"/>
+      <c r="A7" s="44"/>
+      <c r="B7" s="52"/>
       <c r="C7" s="24" t="s">
         <v>9</v>
       </c>
@@ -1376,7 +1403,7 @@
       <c r="E7" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="24" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="8" t="s">
@@ -1422,16 +1449,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="35"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="47"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1617,17 +1644,17 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A12" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="27">
-        <v>44287</v>
-      </c>
-      <c r="C12" s="23"/>
+        <v>59</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
-      <c r="H12" s="15"/>
+      <c r="H12" s="29"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1665,16 +1692,16 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A13" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="21"/>
+      <c r="A13" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="27">
+        <v>44287</v>
+      </c>
+      <c r="C13" s="23"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="14"/>
-      <c r="F13" s="23"/>
+      <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="15"/>
       <c r="I13"/>
@@ -1714,18 +1741,18 @@
       <c r="AQ13"/>
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A14" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="27" t="s">
-        <v>52</v>
+      <c r="A14" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>37</v>
       </c>
       <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
+      <c r="D14" s="21"/>
       <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
+      <c r="F14" s="23"/>
       <c r="G14" s="14"/>
-      <c r="H14" s="29"/>
+      <c r="H14" s="15"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1763,18 +1790,18 @@
       <c r="AQ14"/>
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="27" t="s">
         <v>51</v>
-      </c>
-      <c r="B15" s="27">
-        <v>44621</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
-      <c r="F15" s="23"/>
+      <c r="F15" s="14"/>
       <c r="G15" s="14"/>
-      <c r="H15" s="15"/>
+      <c r="H15" s="29"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1813,16 +1840,16 @@
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A16" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="B16" s="27">
+        <v>44621</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
       <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
+      <c r="G16" s="14"/>
       <c r="H16" s="15"/>
       <c r="I16"/>
       <c r="J16"/>
@@ -1862,15 +1889,15 @@
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A17" s="11" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="B17" s="27">
         <v>44621</v>
       </c>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="15"/>
       <c r="I17"/>
@@ -1910,8 +1937,8 @@
       <c r="AQ17"/>
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A18" s="11" t="s">
-        <v>40</v>
+      <c r="A18" s="26" t="s">
+        <v>60</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>41</v>
@@ -1958,17 +1985,19 @@
       <c r="AP18"/>
       <c r="AQ18"/>
     </row>
-    <row r="19" spans="1:43" s="2" customFormat="1" ht="18">
-      <c r="A19" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="38"/>
+    <row r="19" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A19" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="15"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -2007,15 +2036,15 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A20" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="25"/>
+        <v>39</v>
+      </c>
+      <c r="B20" s="27">
+        <v>44621</v>
+      </c>
+      <c r="C20" s="14"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
-      <c r="F20" s="25"/>
+      <c r="F20" s="23"/>
       <c r="G20" s="14"/>
       <c r="H20" s="15"/>
       <c r="I20"/>
@@ -2056,16 +2085,16 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A21" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="25"/>
+        <v>55</v>
+      </c>
+      <c r="B21" s="27">
+        <v>44287</v>
+      </c>
+      <c r="C21" s="23"/>
       <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="25"/>
       <c r="H21" s="15"/>
       <c r="I21"/>
       <c r="J21"/>
@@ -2105,17 +2134,17 @@
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A22" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>28</v>
+        <v>40</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
       <c r="G22" s="14"/>
-      <c r="H22" s="15"/>
+      <c r="H22" s="29"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -2152,19 +2181,17 @@
       <c r="AP22"/>
       <c r="AQ22"/>
     </row>
-    <row r="23" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A23" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="25"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="15"/>
+    <row r="23" spans="1:43" s="2" customFormat="1" ht="18">
+      <c r="A23" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="50"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -2203,16 +2230,16 @@
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A24" s="11" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B24" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="14"/>
+      <c r="C24" s="25"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
-      <c r="G24" s="25"/>
+      <c r="G24" s="14"/>
       <c r="H24" s="15"/>
       <c r="I24"/>
       <c r="J24"/>
@@ -2252,17 +2279,17 @@
     </row>
     <row r="25" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A25" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B25" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="14"/>
+      <c r="C25" s="25"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
-      <c r="H25" s="29"/>
+      <c r="H25" s="15"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -2299,17 +2326,19 @@
       <c r="AP25"/>
       <c r="AQ25"/>
     </row>
-    <row r="26" spans="1:43" s="2" customFormat="1" ht="18">
-      <c r="A26" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="38"/>
+    <row r="26" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A26" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="15"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2348,15 +2377,15 @@
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A27" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="25"/>
+        <v>62</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="14"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
+      <c r="F27" s="25"/>
       <c r="G27" s="14"/>
       <c r="H27" s="15"/>
       <c r="I27"/>
@@ -2397,15 +2426,15 @@
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A28" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="25"/>
+        <v>44</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="25"/>
+      <c r="D28" s="14"/>
       <c r="E28" s="14"/>
-      <c r="F28" s="21"/>
+      <c r="F28" s="14"/>
       <c r="G28" s="14"/>
       <c r="H28" s="15"/>
       <c r="I28"/>
@@ -2446,17 +2475,17 @@
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A29" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="25"/>
+        <v>56</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="14"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
-      <c r="H29" s="15"/>
+      <c r="H29" s="33"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
@@ -2494,18 +2523,18 @@
       <c r="AQ29"/>
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A30" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="53">
-        <v>44562</v>
-      </c>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="54"/>
-      <c r="H30" s="55"/>
+      <c r="A30" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="15"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -2543,14 +2572,18 @@
       <c r="AQ30"/>
     </row>
     <row r="31" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A31"/>
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="G31"/>
-      <c r="H31"/>
+      <c r="A31" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="29"/>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
@@ -2587,15 +2620,17 @@
       <c r="AP31"/>
       <c r="AQ31"/>
     </row>
-    <row r="32" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A32"/>
-      <c r="B32"/>
-      <c r="C32"/>
-      <c r="D32"/>
-      <c r="E32"/>
-      <c r="F32"/>
-      <c r="G32"/>
-      <c r="H32"/>
+    <row r="32" spans="1:43" s="2" customFormat="1" ht="18">
+      <c r="A32" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="50"/>
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
@@ -2633,14 +2668,18 @@
       <c r="AQ32"/>
     </row>
     <row r="33" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33"/>
-      <c r="D33"/>
-      <c r="E33"/>
-      <c r="F33"/>
-      <c r="G33"/>
-      <c r="H33"/>
+      <c r="A33" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="25"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="15"/>
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
@@ -2677,15 +2716,19 @@
       <c r="AP33"/>
       <c r="AQ33"/>
     </row>
-    <row r="34" spans="1:43" s="2" customFormat="1" ht="15">
-      <c r="A34" s="5"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
+    <row r="34" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A34" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="15"/>
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
@@ -2722,15 +2765,431 @@
       <c r="AP34"/>
       <c r="AQ34"/>
     </row>
-    <row r="35" spans="1:43" customFormat="1"/>
-    <row r="36" spans="1:43" customFormat="1"/>
-    <row r="37" spans="1:43" customFormat="1"/>
-    <row r="38" spans="1:43" customFormat="1"/>
-    <row r="39" spans="1:43" customFormat="1"/>
-    <row r="40" spans="1:43" customFormat="1"/>
-    <row r="41" spans="1:43" customFormat="1"/>
-    <row r="42" spans="1:43" customFormat="1"/>
-    <row r="43" spans="1:43" customFormat="1"/>
+    <row r="35" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A35" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="33"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+      <c r="R35"/>
+      <c r="S35"/>
+      <c r="T35"/>
+      <c r="U35"/>
+      <c r="V35"/>
+      <c r="W35"/>
+      <c r="X35"/>
+      <c r="Y35"/>
+      <c r="Z35"/>
+      <c r="AA35"/>
+      <c r="AB35"/>
+      <c r="AC35"/>
+      <c r="AD35"/>
+      <c r="AE35"/>
+      <c r="AF35"/>
+      <c r="AG35"/>
+      <c r="AH35"/>
+      <c r="AI35"/>
+      <c r="AJ35"/>
+      <c r="AK35"/>
+      <c r="AL35"/>
+      <c r="AM35"/>
+      <c r="AN35"/>
+      <c r="AO35"/>
+      <c r="AP35"/>
+      <c r="AQ35"/>
+    </row>
+    <row r="36" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A36" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="25"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="15"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36"/>
+      <c r="U36"/>
+      <c r="V36"/>
+      <c r="W36"/>
+      <c r="X36"/>
+      <c r="Y36"/>
+      <c r="Z36"/>
+      <c r="AA36"/>
+      <c r="AB36"/>
+      <c r="AC36"/>
+      <c r="AD36"/>
+      <c r="AE36"/>
+      <c r="AF36"/>
+      <c r="AG36"/>
+      <c r="AH36"/>
+      <c r="AI36"/>
+      <c r="AJ36"/>
+      <c r="AK36"/>
+      <c r="AL36"/>
+      <c r="AM36"/>
+      <c r="AN36"/>
+      <c r="AO36"/>
+      <c r="AP36"/>
+      <c r="AQ36"/>
+    </row>
+    <row r="37" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A37" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="15"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+      <c r="S37"/>
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
+      <c r="X37"/>
+      <c r="Y37"/>
+      <c r="Z37"/>
+      <c r="AA37"/>
+      <c r="AB37"/>
+      <c r="AC37"/>
+      <c r="AD37"/>
+      <c r="AE37"/>
+      <c r="AF37"/>
+      <c r="AG37"/>
+      <c r="AH37"/>
+      <c r="AI37"/>
+      <c r="AJ37"/>
+      <c r="AK37"/>
+      <c r="AL37"/>
+      <c r="AM37"/>
+      <c r="AN37"/>
+      <c r="AO37"/>
+      <c r="AP37"/>
+      <c r="AQ37"/>
+    </row>
+    <row r="38" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A38" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="15"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38"/>
+      <c r="P38"/>
+      <c r="Q38"/>
+      <c r="R38"/>
+      <c r="S38"/>
+      <c r="T38"/>
+      <c r="U38"/>
+      <c r="V38"/>
+      <c r="W38"/>
+      <c r="X38"/>
+      <c r="Y38"/>
+      <c r="Z38"/>
+      <c r="AA38"/>
+      <c r="AB38"/>
+      <c r="AC38"/>
+      <c r="AD38"/>
+      <c r="AE38"/>
+      <c r="AF38"/>
+      <c r="AG38"/>
+      <c r="AH38"/>
+      <c r="AI38"/>
+      <c r="AJ38"/>
+      <c r="AK38"/>
+      <c r="AL38"/>
+      <c r="AM38"/>
+      <c r="AN38"/>
+      <c r="AO38"/>
+      <c r="AP38"/>
+      <c r="AQ38"/>
+    </row>
+    <row r="39" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A39" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" s="31">
+        <v>44562</v>
+      </c>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="33"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+      <c r="N39"/>
+      <c r="O39"/>
+      <c r="P39"/>
+      <c r="Q39"/>
+      <c r="R39"/>
+      <c r="S39"/>
+      <c r="T39"/>
+      <c r="U39"/>
+      <c r="V39"/>
+      <c r="W39"/>
+      <c r="X39"/>
+      <c r="Y39"/>
+      <c r="Z39"/>
+      <c r="AA39"/>
+      <c r="AB39"/>
+      <c r="AC39"/>
+      <c r="AD39"/>
+      <c r="AE39"/>
+      <c r="AF39"/>
+      <c r="AG39"/>
+      <c r="AH39"/>
+      <c r="AI39"/>
+      <c r="AJ39"/>
+      <c r="AK39"/>
+      <c r="AL39"/>
+      <c r="AM39"/>
+      <c r="AN39"/>
+      <c r="AO39"/>
+      <c r="AP39"/>
+      <c r="AQ39"/>
+    </row>
+    <row r="40" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A40"/>
+      <c r="B40"/>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+      <c r="N40"/>
+      <c r="O40"/>
+      <c r="P40"/>
+      <c r="Q40"/>
+      <c r="R40"/>
+      <c r="S40"/>
+      <c r="T40"/>
+      <c r="U40"/>
+      <c r="V40"/>
+      <c r="W40"/>
+      <c r="X40"/>
+      <c r="Y40"/>
+      <c r="Z40"/>
+      <c r="AA40"/>
+      <c r="AB40"/>
+      <c r="AC40"/>
+      <c r="AD40"/>
+      <c r="AE40"/>
+      <c r="AF40"/>
+      <c r="AG40"/>
+      <c r="AH40"/>
+      <c r="AI40"/>
+      <c r="AJ40"/>
+      <c r="AK40"/>
+      <c r="AL40"/>
+      <c r="AM40"/>
+      <c r="AN40"/>
+      <c r="AO40"/>
+      <c r="AP40"/>
+      <c r="AQ40"/>
+    </row>
+    <row r="41" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A41"/>
+      <c r="B41"/>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41"/>
+      <c r="O41"/>
+      <c r="P41"/>
+      <c r="Q41"/>
+      <c r="R41"/>
+      <c r="S41"/>
+      <c r="T41"/>
+      <c r="U41"/>
+      <c r="V41"/>
+      <c r="W41"/>
+      <c r="X41"/>
+      <c r="Y41"/>
+      <c r="Z41"/>
+      <c r="AA41"/>
+      <c r="AB41"/>
+      <c r="AC41"/>
+      <c r="AD41"/>
+      <c r="AE41"/>
+      <c r="AF41"/>
+      <c r="AG41"/>
+      <c r="AH41"/>
+      <c r="AI41"/>
+      <c r="AJ41"/>
+      <c r="AK41"/>
+      <c r="AL41"/>
+      <c r="AM41"/>
+      <c r="AN41"/>
+      <c r="AO41"/>
+      <c r="AP41"/>
+      <c r="AQ41"/>
+    </row>
+    <row r="42" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
+      <c r="A42"/>
+      <c r="B42"/>
+      <c r="C42"/>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+      <c r="L42"/>
+      <c r="M42"/>
+      <c r="N42"/>
+      <c r="O42"/>
+      <c r="P42"/>
+      <c r="Q42"/>
+      <c r="R42"/>
+      <c r="S42"/>
+      <c r="T42"/>
+      <c r="U42"/>
+      <c r="V42"/>
+      <c r="W42"/>
+      <c r="X42"/>
+      <c r="Y42"/>
+      <c r="Z42"/>
+      <c r="AA42"/>
+      <c r="AB42"/>
+      <c r="AC42"/>
+      <c r="AD42"/>
+      <c r="AE42"/>
+      <c r="AF42"/>
+      <c r="AG42"/>
+      <c r="AH42"/>
+      <c r="AI42"/>
+      <c r="AJ42"/>
+      <c r="AK42"/>
+      <c r="AL42"/>
+      <c r="AM42"/>
+      <c r="AN42"/>
+      <c r="AO42"/>
+      <c r="AP42"/>
+      <c r="AQ42"/>
+    </row>
+    <row r="43" spans="1:43" s="2" customFormat="1" ht="15">
+      <c r="A43" s="5"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43"/>
+      <c r="J43"/>
+      <c r="K43"/>
+      <c r="L43"/>
+      <c r="M43"/>
+      <c r="N43"/>
+      <c r="O43"/>
+      <c r="P43"/>
+      <c r="Q43"/>
+      <c r="R43"/>
+      <c r="S43"/>
+      <c r="T43"/>
+      <c r="U43"/>
+      <c r="V43"/>
+      <c r="W43"/>
+      <c r="X43"/>
+      <c r="Y43"/>
+      <c r="Z43"/>
+      <c r="AA43"/>
+      <c r="AB43"/>
+      <c r="AC43"/>
+      <c r="AD43"/>
+      <c r="AE43"/>
+      <c r="AF43"/>
+      <c r="AG43"/>
+      <c r="AH43"/>
+      <c r="AI43"/>
+      <c r="AJ43"/>
+      <c r="AK43"/>
+      <c r="AL43"/>
+      <c r="AM43"/>
+      <c r="AN43"/>
+      <c r="AO43"/>
+      <c r="AP43"/>
+      <c r="AQ43"/>
+    </row>
     <row r="44" spans="1:43" customFormat="1"/>
     <row r="45" spans="1:43" customFormat="1"/>
     <row r="46" spans="1:43" customFormat="1"/>
@@ -2768,20 +3227,29 @@
     <row r="78" customFormat="1"/>
     <row r="79" customFormat="1"/>
     <row r="80" customFormat="1"/>
+    <row r="81" customFormat="1"/>
+    <row r="82" customFormat="1"/>
+    <row r="83" customFormat="1"/>
+    <row r="84" customFormat="1"/>
+    <row r="85" customFormat="1"/>
+    <row r="86" customFormat="1"/>
+    <row r="87" customFormat="1"/>
+    <row r="88" customFormat="1"/>
+    <row r="89" customFormat="1"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A5:H5"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="F3:H3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A5:H5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>